<commit_message>
update webCrawling project files
</commit_message>
<xml_diff>
--- a/Python WebCrawling/yungum.xlsx
+++ b/Python WebCrawling/yungum.xlsx
@@ -424,7 +424,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>노령연금 입금금액 = 90000</t>
+          <t>노령연금 입금금액 = 330000</t>
         </is>
       </c>
     </row>
@@ -468,37 +468,37 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>188,910</t>
+          <t>325,920</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>280,960</t>
+          <t>484,710</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>373,000</t>
+          <t>643,500</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>465,040</t>
+          <t>802,300</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>557,090</t>
+          <t>961,090</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>649,130</t>
+          <t>1,119,880</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>741,170</t>
+          <t>1,278,680</t>
         </is>
       </c>
     </row>

</xml_diff>